<commit_message>
Provide service to upload spreadsheets; rename ContactRowHandler to ContactImport
</commit_message>
<xml_diff>
--- a/backend/fixture/src/main/java/domainapp/fixture/scenarios/demo/DemoFixture.xlsx
+++ b/backend/fixture/src/main/java/domainapp/fixture/scenarios/demo/DemoFixture.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvanderwal\src\github\incodehq\contactapp\fixture\src\main\java\domainapp\fixture\scenarios\demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jvanderwal/src/github/incodehq/contactapp/backend/fixture/src/main/java/domainapp/fixture/scenarios/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="26832" windowHeight="13116"/>
+    <workbookView xWindow="-1800" yWindow="-25720" windowWidth="34620" windowHeight="16660"/>
   </bookViews>
   <sheets>
-    <sheet name="ContactRowHandler" sheetId="5" r:id="rId1"/>
+    <sheet name="ContactImport" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -479,9 +484,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -514,9 +519,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -723,12 +728,12 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="49.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="18" bestFit="1" customWidth="1"/>
@@ -737,7 +742,7 @@
     <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -769,7 +774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>78</v>
       </c>
@@ -795,7 +800,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
@@ -815,7 +820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
@@ -837,7 +842,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -855,7 +860,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>38</v>
       </c>
@@ -874,7 +879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>22</v>
       </c>
@@ -892,7 +897,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D8" s="4" t="s">
         <v>48</v>
       </c>
@@ -907,7 +912,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -931,7 +936,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>77</v>
       </c>
@@ -949,7 +954,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>80</v>
       </c>
@@ -971,7 +976,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12" s="7" t="s">
         <v>59</v>
       </c>
@@ -992,7 +997,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C13" s="7" t="s">
         <v>60</v>
       </c>
@@ -1013,7 +1018,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C14" s="7" t="s">
         <v>58</v>
       </c>
@@ -1030,7 +1035,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C15" s="7" t="s">
         <v>20</v>
       </c>

</xml_diff>